<commit_message>
Add sheet name filter
</commit_message>
<xml_diff>
--- a/core/src/test/resources/contains_formula.xlsx
+++ b/core/src/test/resources/contains_formula.xlsx
@@ -20,45 +20,29 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t xml:space="preserve">a</t>
+    <t xml:space="preserve">AAA</t>
   </si>
   <si>
-    <t xml:space="preserve">b</t>
+    <t xml:space="preserve">甲</t>
   </si>
   <si>
-    <t xml:space="preserve">c</t>
-  </si>
-  <si>
-    <t xml:space="preserve">d</t>
-  </si>
-  <si>
-    <t xml:space="preserve">e</t>
-  </si>
-  <si>
-    <t xml:space="preserve">f</t>
-  </si>
-  <si>
-    <t xml:space="preserve">g</t>
-  </si>
-  <si>
-    <t xml:space="preserve">h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">i</t>
+    <t xml:space="preserve">x</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
-    <numFmt numFmtId="166" formatCode="General"/>
+    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="167" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+    <numFmt numFmtId="168" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -79,6 +63,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="PingFang SC"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -123,7 +113,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -137,6 +127,18 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -153,70 +155,115 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
+      <c r="A1" s="1" t="str">
+        <f aca="false">CHAR(96+COLUMN())</f>
+        <v>a</v>
+      </c>
+      <c r="B1" s="1" t="str">
+        <f aca="false">CHAR(96+COLUMN())</f>
+        <v>b</v>
+      </c>
+      <c r="C1" s="1" t="str">
+        <f aca="false">CHAR(96+COLUMN())</f>
+        <v>c</v>
+      </c>
+      <c r="D1" s="1" t="str">
+        <f aca="false">CHAR(96+COLUMN())</f>
+        <v>d</v>
+      </c>
+      <c r="E1" s="1" t="str">
+        <f aca="false">CHAR(96+COLUMN())</f>
+        <v>e</v>
+      </c>
+      <c r="F1" s="1" t="str">
+        <f aca="false">CHAR(96+COLUMN())</f>
+        <v>f</v>
+      </c>
+      <c r="G1" s="1" t="str">
+        <f aca="false">CHAR(96+COLUMN())</f>
+        <v>g</v>
+      </c>
+      <c r="H1" s="1" t="str">
+        <f aca="false">CHAR(96+COLUMN())</f>
+        <v>h</v>
+      </c>
+      <c r="I1" s="1" t="str">
+        <f aca="false">CHAR(96+COLUMN())</f>
+        <v>i</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
-        <f aca="false">COLUMN()*10</f>
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="B2" s="1" t="n">
-        <f aca="false">A2+11</f>
-        <v>21</v>
+        <v>10000000000</v>
       </c>
       <c r="C2" s="1" t="n">
-        <f aca="false">B2/2</f>
-        <v>10.5</v>
+        <v>0.5</v>
       </c>
       <c r="D2" s="2" t="n">
-        <f aca="false">DATE(2019,A2,B2)</f>
-        <v>43759</v>
-      </c>
-      <c r="F2" s="1" t="str">
-        <f aca="false">A1&amp;B1&amp;C1</f>
-        <v>abc</v>
-      </c>
-      <c r="H2" s="3" t="n">
-        <f aca="false">A2=B2</f>
+        <v>43800</v>
+      </c>
+      <c r="E2" s="3" t="n">
+        <v>43800.395844919</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="n">
+        <f aca="false">A2+100</f>
+        <v>200</v>
+      </c>
+      <c r="B3" s="1" t="n">
+        <f aca="false">B2+10000000000</f>
+        <v>20000000000</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <f aca="false">C2/2</f>
+        <v>0.25</v>
+      </c>
+      <c r="D3" s="2" t="n">
+        <f aca="false">D2+1</f>
+        <v>43801</v>
+      </c>
+      <c r="E3" s="3" t="n">
+        <v>43801.3958565046</v>
+      </c>
+      <c r="F3" s="1" t="str">
+        <f aca="false">"BBB"</f>
+        <v>BBB</v>
+      </c>
+      <c r="G3" s="4" t="str">
+        <f aca="false">"乙"</f>
+        <v>乙</v>
+      </c>
+      <c r="H3" s="6" t="n">
+        <f aca="false">NOT(H2)</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>